<commit_message>
test working in 2 and 3
</commit_message>
<xml_diff>
--- a/tests/test_one.xlsx
+++ b/tests/test_one.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t xml:space="preserve">a</t>
   </si>
@@ -38,7 +38,7 @@
     <t xml:space="preserve">space field</t>
   </si>
   <si>
-    <t xml:space="preserve">”(* really odd field ☺ *)”</t>
+    <t xml:space="preserve">(* really odd field ☺ *)</t>
   </si>
   <si>
     <t xml:space="preserve">not a number</t>
@@ -50,6 +50,9 @@
     <t xml:space="preserve">12.3.2</t>
   </si>
   <si>
+    <t xml:space="preserve">☺ unicode ☺</t>
+  </si>
+  <si>
     <t xml:space="preserve">sum</t>
   </si>
   <si>
@@ -59,10 +62,10 @@
     <t xml:space="preserve">sumsq</t>
   </si>
   <si>
-    <t xml:space="preserve">varianceX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stdX</t>
+    <t xml:space="preserve">variance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">std</t>
   </si>
   <si>
     <t xml:space="preserve">min</t>
@@ -74,7 +77,7 @@
     <t xml:space="preserve">n</t>
   </si>
   <si>
-    <t xml:space="preserve">coefvarX</t>
+    <t xml:space="preserve">coefvar</t>
   </si>
 </sst>
 </file>
@@ -85,7 +88,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -106,6 +109,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,12 +158,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -183,9 +195,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -568,8 +577,8 @@
       <c r="D20" s="0" t="n">
         <v>0.0380568375149319</v>
       </c>
-      <c r="F20" s="0" t="n">
-        <v>18</v>
+      <c r="F20" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,13 +617,10 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -639,10 +645,10 @@
       </c>
       <c r="F1" s="0" t="n">
         <f aca="false">SUM(Sheet1!F$2:F$21)</f>
-        <v>10000000160</v>
+        <v>10000000142</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,10 +674,10 @@
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">AVERAGE(Sheet1!F$2:F$21)</f>
-        <v>555555564.444444</v>
+        <v>588235302.470588</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -700,7 +706,7 @@
         <v>1E+020</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,10 +732,10 @@
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">VARPA(Sheet1!F$2:F$21)</f>
-        <v>4.749999992E+018</v>
+        <v>4.7499999929E+018</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,10 +761,10 @@
       </c>
       <c r="F5" s="0" t="n">
         <f aca="false">SQRT(F4)</f>
-        <v>2179449469.93501</v>
+        <v>2179449470.14149</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,7 +793,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -816,7 +822,7 @@
         <v>10000000000</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,10 +848,10 @@
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">COUNT(Sheet1!F$2:F$21)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -871,10 +877,10 @@
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">F5/F2</f>
-        <v>3.92300898311488</v>
+        <v>3.70506404662862</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>